<commit_message>
Doku fuer Solarposition erweitert
</commit_message>
<xml_diff>
--- a/ST_Team_1.xlsx
+++ b/ST_Team_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SynologyDrive\Dokumente\HAW\9_Sensortechnik\doc-report-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9D3A8F-A63D-4E28-B3C9-A6A88F9085F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C5CC35-D4F8-469A-BE13-C1F2E9A2DEE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-1905" windowWidth="19440" windowHeight="15000" xr2:uid="{AEF30A94-AB2F-4F44-9FB2-2DBCA6CB05FB}"/>
+    <workbookView xWindow="39180" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{AEF30A94-AB2F-4F44-9FB2-2DBCA6CB05FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabenverteilung" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B0B1B5-79EE-4ABD-8AE7-228241FBE244}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
       <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="10" t="s">
@@ -832,9 +832,9 @@
       <c r="C19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="10" t="s">
         <v>38</v>
       </c>

</xml_diff>